<commit_message>
Units added to the final report
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -400,7 +400,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,7 +432,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -443,7 +443,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Logger improved, Logo Added to GUI
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Site</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>566-P-2927</t>
   </si>
   <si>
     <t>Result</t>
@@ -397,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +418,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -432,7 +429,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -444,17 +441,6 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor code and fix formatting issues
</commit_message>
<xml_diff>
--- a/TaskList.xlsx
+++ b/TaskList.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{977187AB-6E46-4829-A049-523F1B49FD51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A87D468F-CBF9-440F-8E2E-1C6A31C9611D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_list_1" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="74">
   <si>
     <t>Site</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Success</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -624,7 +630,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -727,9 +733,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -751,9 +755,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -775,9 +777,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
@@ -799,9 +799,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -823,9 +821,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -847,9 +843,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -871,9 +865,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -895,9 +887,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -919,9 +909,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -943,9 +931,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -967,9 +953,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -1034,9 +1018,11 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
@@ -1060,17 +1046,35 @@
       <c r="D16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2662</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1767</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.3</v>
+      </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="3"/>
+      <c r="J16" s="2">
+        <v>-69</v>
+      </c>
+      <c r="K16" s="2">
+        <v>4388</v>
+      </c>
+      <c r="L16" s="2">
+        <v>2914</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.49</v>
+      </c>
       <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2">
+        <v>86</v>
+      </c>
       <c r="P16" s="1"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -1081,9 +1085,7 @@
         <v>55</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1105,9 +1107,7 @@
         <v>56</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1525,9 +1525,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1549,9 +1547,7 @@
         <v>42</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -1573,9 +1569,7 @@
         <v>50</v>
       </c>
       <c r="C39" s="1"/>
-      <c r="D39" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -1597,9 +1591,7 @@
         <v>43</v>
       </c>
       <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1621,9 +1613,7 @@
         <v>44</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -1645,9 +1635,7 @@
         <v>45</v>
       </c>
       <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -1669,9 +1657,7 @@
         <v>51</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -1693,9 +1679,7 @@
         <v>47</v>
       </c>
       <c r="C44" s="1"/>
-      <c r="D44" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -1717,9 +1701,7 @@
         <v>48</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -1741,9 +1723,7 @@
         <v>49</v>
       </c>
       <c r="C46" s="1"/>
-      <c r="D46" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -1765,9 +1745,7 @@
         <v>52</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -1789,9 +1767,7 @@
         <v>53</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>

</xml_diff>